<commit_message>
GITBOOK-67: Holli - Mob Heads - File updated
</commit_message>
<xml_diff>
--- a/.gitbook/assets/Mob_Head_Collection_List_S3.xlsx
+++ b/.gitbook/assets/Mob_Head_Collection_List_S3.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11310"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10635" windowHeight="5910"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="189">
   <si>
     <t>Variant 1</t>
   </si>
@@ -1069,6 +1069,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1080,12 +1086,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3220,7 +3220,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp479.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H92" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3228,15 +3228,19 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp480.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E43" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp481.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E43" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E44" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp482.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E44" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H92" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp483.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H88" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp49.xml><?xml version="1.0" encoding="utf-8"?>
@@ -34187,14 +34191,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>90</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="209550"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>92</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1541" name="Check Box 517" hidden="1">
@@ -34240,7 +34249,71 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor editAs="oneCell">
+        <xdr:from>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>28575</xdr:colOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>171450</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>3</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>44</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="1542" name="Check Box 518" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s1542"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:extLst>
+              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+                <a14:hiddenFill>
+                  <a:solidFill>
+                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
+                  </a:solidFill>
+                </a14:hiddenFill>
+              </a:ext>
+              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
+                <a14:hiddenLine w="9525">
+                  <a:solidFill>
+                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
+                  </a:solidFill>
+                  <a:miter lim="800000"/>
+                  <a:headEnd/>
+                  <a:tailEnd/>
+                </a14:hiddenLine>
+              </a:ext>
+            </a:extLst>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -34248,18 +34321,18 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:oneCellAnchor>
         <xdr:from>
-          <xdr:col>3</xdr:col>
+          <xdr:col>6</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>42</xdr:row>
+          <xdr:row>86</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:ext cx="228600" cy="209550"/>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
-            <xdr:cNvPr id="1542" name="Check Box 518" hidden="1">
+            <xdr:cNvPr id="1543" name="Check Box 519" hidden="1">
               <a:extLst>
                 <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1542"/>
+                  <a14:compatExt spid="_x0000_s1543"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -34627,7 +34700,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -34693,7 +34766,7 @@
       </c>
       <c r="B3" s="16">
         <f>COUNTIFS(E:AI,FALSE)</f>
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="AJ3">
         <v>0.1</v>
@@ -34728,50 +34801,50 @@
       <c r="B7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="24" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="F7" s="28" t="s">
+      <c r="D7" s="25"/>
+      <c r="F7" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="29"/>
-      <c r="I7" s="28" t="s">
+      <c r="G7" s="25"/>
+      <c r="I7" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="29"/>
-      <c r="L7" s="28" t="s">
+      <c r="J7" s="25"/>
+      <c r="L7" s="24" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="29"/>
-      <c r="O7" s="28" t="s">
+      <c r="M7" s="25"/>
+      <c r="O7" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="P7" s="29"/>
-      <c r="R7" s="28" t="s">
+      <c r="P7" s="25"/>
+      <c r="R7" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="29"/>
-      <c r="U7" s="28" t="s">
+      <c r="S7" s="25"/>
+      <c r="U7" s="24" t="s">
         <v>93</v>
       </c>
-      <c r="V7" s="29"/>
-      <c r="X7" s="28" t="s">
+      <c r="V7" s="25"/>
+      <c r="X7" s="24" t="s">
         <v>94</v>
       </c>
-      <c r="Y7" s="29"/>
-      <c r="AA7" s="28" t="s">
+      <c r="Y7" s="25"/>
+      <c r="AA7" s="24" t="s">
         <v>95</v>
       </c>
-      <c r="AB7" s="29"/>
-      <c r="AD7" s="28" t="s">
+      <c r="AB7" s="25"/>
+      <c r="AD7" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="AE7" s="29"/>
-      <c r="AG7" s="28" t="s">
+      <c r="AE7" s="25"/>
+      <c r="AG7" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="AH7" s="29"/>
+      <c r="AH7" s="25"/>
       <c r="AJ7">
         <v>0.3</v>
       </c>
@@ -36068,10 +36141,10 @@
       <c r="AH36" s="5"/>
     </row>
     <row r="37" spans="1:34">
-      <c r="A37" s="24" t="s">
+      <c r="A37" s="26" t="s">
         <v>186</v>
       </c>
-      <c r="B37" s="26" t="s">
+      <c r="B37" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -36138,8 +36211,8 @@
       <c r="AH37" s="5"/>
     </row>
     <row r="38" spans="1:34">
-      <c r="A38" s="25"/>
-      <c r="B38" s="27"/>
+      <c r="A38" s="27"/>
+      <c r="B38" s="29"/>
       <c r="C38" s="8" t="s">
         <v>141</v>
       </c>
@@ -37241,10 +37314,10 @@
       <c r="AH61" s="5"/>
     </row>
     <row r="62" spans="1:34">
-      <c r="A62" s="24" t="s">
+      <c r="A62" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="26" t="s">
+      <c r="B62" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -37311,8 +37384,8 @@
       <c r="AH62" s="5"/>
     </row>
     <row r="63" spans="1:34">
-      <c r="A63" s="25"/>
-      <c r="B63" s="27"/>
+      <c r="A63" s="27"/>
+      <c r="B63" s="29"/>
       <c r="C63" s="8" t="s">
         <v>141</v>
       </c>
@@ -37382,10 +37455,10 @@
       <c r="AH63" s="5"/>
     </row>
     <row r="64" spans="1:34">
-      <c r="A64" s="24" t="s">
+      <c r="A64" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="B64" s="26" t="s">
+      <c r="B64" s="28" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="8" t="s">
@@ -37452,8 +37525,8 @@
       <c r="AH64" s="5"/>
     </row>
     <row r="65" spans="1:34">
-      <c r="A65" s="25"/>
-      <c r="B65" s="27"/>
+      <c r="A65" s="27"/>
+      <c r="B65" s="29"/>
       <c r="C65" s="8" t="s">
         <v>141</v>
       </c>
@@ -38132,10 +38205,10 @@
       <c r="AH80" s="5"/>
     </row>
     <row r="81" spans="1:34">
-      <c r="A81" s="24" t="s">
+      <c r="A81" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="B81" s="26" t="s">
+      <c r="B81" s="28" t="s">
         <v>38</v>
       </c>
       <c r="C81" s="8" t="s">
@@ -38202,8 +38275,8 @@
       <c r="AH81" s="5"/>
     </row>
     <row r="82" spans="1:34">
-      <c r="A82" s="25"/>
-      <c r="B82" s="27"/>
+      <c r="A82" s="27"/>
+      <c r="B82" s="29"/>
       <c r="C82" s="8" t="s">
         <v>149</v>
       </c>
@@ -38479,9 +38552,13 @@
       <c r="E88" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F88" s="8"/>
+      <c r="F88" s="8" t="s">
+        <v>187</v>
+      </c>
       <c r="G88" s="5"/>
-      <c r="H88" s="1"/>
+      <c r="H88" s="1" t="b">
+        <v>0</v>
+      </c>
       <c r="I88" s="8"/>
       <c r="J88" s="5"/>
       <c r="K88" s="1"/>
@@ -38505,10 +38582,10 @@
       <c r="AH88" s="5"/>
     </row>
     <row r="89" spans="1:34">
-      <c r="A89" s="24" t="s">
+      <c r="A89" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="B89" s="26" t="s">
+      <c r="B89" s="28" t="s">
         <v>58</v>
       </c>
       <c r="C89" s="8" t="s">
@@ -38580,8 +38657,8 @@
       <c r="AH89" s="5"/>
     </row>
     <row r="90" spans="1:34">
-      <c r="A90" s="25"/>
-      <c r="B90" s="27"/>
+      <c r="A90" s="27"/>
+      <c r="B90" s="29"/>
       <c r="C90" s="8" t="s">
         <v>92</v>
       </c>
@@ -38772,10 +38849,10 @@
       <c r="AH93" s="5"/>
     </row>
     <row r="94" spans="1:34">
-      <c r="A94" s="24" t="s">
+      <c r="A94" s="26" t="s">
         <v>84</v>
       </c>
-      <c r="B94" s="26" t="s">
+      <c r="B94" s="28" t="s">
         <v>59</v>
       </c>
       <c r="C94" s="8" t="s">
@@ -38842,8 +38919,8 @@
       <c r="AH94" s="5"/>
     </row>
     <row r="95" spans="1:34">
-      <c r="A95" s="25"/>
-      <c r="B95" s="27"/>
+      <c r="A95" s="27"/>
+      <c r="B95" s="29"/>
       <c r="C95" s="8" t="s">
         <v>149</v>
       </c>
@@ -38943,6 +39020,15 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
     <mergeCell ref="X7:Y7"/>
     <mergeCell ref="AA7:AB7"/>
     <mergeCell ref="AD7:AE7"/>
@@ -38957,15 +39043,6 @@
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="A37:A38"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C96">
     <cfRule type="expression" dxfId="38" priority="39">
@@ -49647,7 +49724,73 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1541" r:id="rId482" name="Check Box 517">
+            <control shapeId="1099" r:id="rId482" name="Check Box 75">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>40</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:row>42</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1100" r:id="rId483" name="Check Box 76">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>41</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:row>43</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1542" r:id="rId484" name="Check Box 518">
+              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
+                <anchor moveWithCells="1">
+                  <from>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>28575</xdr:colOff>
+                    <xdr:row>42</xdr:row>
+                    <xdr:rowOff>171450</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>3</xdr:col>
+                    <xdr:colOff>257175</xdr:colOff>
+                    <xdr:row>44</xdr:row>
+                    <xdr:rowOff>19050</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="1541" r:id="rId485" name="Check Box 517">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49669,63 +49812,19 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1099" r:id="rId483" name="Check Box 75">
+            <control shapeId="1543" r:id="rId486" name="Check Box 519">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>40</xdr:row>
+                    <xdr:row>86</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>3</xdr:col>
+                    <xdr:col>6</xdr:col>
                     <xdr:colOff>257175</xdr:colOff>
-                    <xdr:row>42</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1100" r:id="rId484" name="Check Box 76">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>41</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
-                    <xdr:row>43</xdr:row>
-                    <xdr:rowOff>19050</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1542" r:id="rId485" name="Check Box 518">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>42</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>3</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
-                    <xdr:row>44</xdr:row>
+                    <xdr:row>88</xdr:row>
                     <xdr:rowOff>19050</xdr:rowOff>
                   </to>
                 </anchor>

</xml_diff>

<commit_message>
GITBOOK-70: Holli - no more allay cookie
</commit_message>
<xml_diff>
--- a/.gitbook/assets/Mob_Head_Collection_List_S3.xlsx
+++ b/.gitbook/assets/Mob_Head_Collection_List_S3.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="582" uniqueCount="188">
   <si>
     <t>Variant 1</t>
   </si>
@@ -566,9 +566,6 @@
     <t>Coffee</t>
   </si>
   <si>
-    <t>Cookie</t>
-  </si>
-  <si>
     <t>Puffed</t>
   </si>
   <si>
@@ -1069,12 +1066,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1086,6 +1077,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2496,23 +2493,23 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp315.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp316.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp317.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp317.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp318.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H58" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp319.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H58" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H71" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp32.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2520,43 +2517,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp320.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H71" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H75" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp321.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H75" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E66" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp322.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E66" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp323.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp324.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp325.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp326.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp327.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp328.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp329.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp33.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2564,43 +2561,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp330.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp331.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp332.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp333.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp334.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp335.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp336.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp337.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp338.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp339.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp34.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2608,43 +2605,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp340.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp341.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp342.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp343.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp344.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp345.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp346.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp347.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z62" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp348.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z62" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp349.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z64" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp35.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2652,43 +2649,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp350.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z64" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H53" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp351.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H53" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H50" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp352.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H50" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H51" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp353.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H51" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K53" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp354.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K53" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K50" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp355.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K50" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K51" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp356.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K51" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp357.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp358.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp359.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E91" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp36.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2696,43 +2693,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp360.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E91" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K89" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp361.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K89" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K86" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp362.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K86" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K90" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp363.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K90" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp364.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp365.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp365.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp366.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N89" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp367.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp368.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp366.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp369.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp367.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N89" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp368.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp369.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp37.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2740,43 +2737,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp370.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N81" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp371.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp371.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N81" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp372.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp372.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp373.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp373.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp374.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N82" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp375.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp376.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp374.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp377.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp375.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N82" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp376.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp377.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp378.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N90" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp379.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N90" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp38.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2784,43 +2781,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp380.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp381.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp381.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp382.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q89" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp383.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp384.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp382.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp385.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp383.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q89" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp386.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q81" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp384.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp387.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp385.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp388.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp386.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp389.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp387.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q81" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp388.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp389.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp39.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2828,43 +2825,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp390.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q82" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp391.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp391.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q82" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp392.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp392.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp393.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp393.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp394.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q90" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp395.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp396.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp394.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp397.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp395.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q90" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp396.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp397.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp398.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T81" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp399.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T81" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2876,43 +2873,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp400.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp401.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp401.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp402.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T82" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp403.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp404.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp402.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp405.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp403.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T82" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp406.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T89" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp404.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp407.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp405.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp408.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp406.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp409.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp407.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T89" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp408.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp409.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp41.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2920,43 +2917,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp410.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T90" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp411.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp411.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T90" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp412.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp412.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp413.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp413.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp414.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W89" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp415.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp416.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp414.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp417.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp415.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W89" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp416.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp417.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp418.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W90" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp419.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W90" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp42.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2964,43 +2961,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp420.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp421.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp421.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp422.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W81" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp423.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp424.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp422.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp425.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp423.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W81" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp426.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W82" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp424.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp427.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp425.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp428.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp426.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp429.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp427.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W82" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp428.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp429.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp43.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3008,43 +3005,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp430.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z81" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp431.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp431.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z81" lockText="1" noThreeD="1"/>
+<file path=xl/ctrlProps/ctrlProp432.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp432.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp433.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp433.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp434.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z89" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp435.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp436.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp434.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp437.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp435.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z89" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp436.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp437.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp438.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z90" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp439.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z90" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC65" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp44.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3052,43 +3049,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp440.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC65" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC89" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp441.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC89" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC90" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp442.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC90" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp443.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E39" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp444.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E39" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp445.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp446.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp447.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp448.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp449.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp45.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3096,43 +3093,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp450.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="K40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp451.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp452.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp453.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="N38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp454.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp455.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp456.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Q38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp457.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp458.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp459.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="T38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W37" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp46.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3140,43 +3137,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp460.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W37" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W40" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp461.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W40" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp462.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="W38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp463.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp464.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp464.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp465.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z37" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp466.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp467.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp465.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/ctrlProps/ctrlProp468.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp466.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z37" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp467.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp468.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp469.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z59" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp47.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3184,43 +3181,43 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp470.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z59" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp471.xml><?xml version="1.0" encoding="utf-8"?>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
+</file>
+
+<file path=xl/ctrlProps/ctrlProp472.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
 </file>
 
-<file path=xl/ctrlProps/ctrlProp472.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E18" lockText="1" noThreeD="1"/>
-</file>
-
 <file path=xl/ctrlProps/ctrlProp473.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="$E$8" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp474.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="Z38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC38" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp475.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC38" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC63" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp476.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="AC63" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H89" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp477.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H89" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H90" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp478.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H90" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E42" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp479.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E42" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E43" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp48.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3228,18 +3225,14 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp480.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E43" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E44" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp481.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="E44" lockText="1" noThreeD="1"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H92" lockText="1" noThreeD="1"/>
 </file>
 
 <file path=xl/ctrlProps/ctrlProp482.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H92" lockText="1" noThreeD="1"/>
-</file>
-
-<file path=xl/ctrlProps/ctrlProp483.xml><?xml version="1.0" encoding="utf-8"?>
 <formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="CheckBox" fmlaLink="H88" lockText="1" noThreeD="1"/>
 </file>
 
@@ -28051,70 +28044,6 @@
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
-          <xdr:row>6</xdr:row>
-          <xdr:rowOff>171450</xdr:rowOff>
-        </xdr:from>
-        <xdr:to>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>257175</xdr:colOff>
-          <xdr:row>8</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
-        </xdr:to>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="1444" name="Check Box 420" hidden="1">
-              <a:extLst>
-                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
-                  <a14:compatExt spid="_x0000_s1444"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr/>
-          </xdr:nvSpPr>
-          <xdr:spPr bwMode="auto">
-            <a:xfrm>
-              <a:off x="0" y="0"/>
-              <a:ext cx="0" cy="0"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:extLst>
-              <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-                <a14:hiddenFill>
-                  <a:solidFill>
-                    <a:srgbClr val="FFFFFF" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="65"/>
-                  </a:solidFill>
-                </a14:hiddenFill>
-              </a:ext>
-              <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-                <a14:hiddenLine w="9525">
-                  <a:solidFill>
-                    <a:srgbClr val="000000" mc:Ignorable="a14" a14:legacySpreadsheetColorIndex="64"/>
-                  </a:solidFill>
-                  <a:miter lim="800000"/>
-                  <a:headEnd/>
-                  <a:tailEnd/>
-                </a14:hiddenLine>
-              </a:ext>
-            </a:extLst>
-          </xdr:spPr>
-        </xdr:sp>
-        <xdr:clientData/>
-      </xdr:twoCellAnchor>
-    </mc:Choice>
-    <mc:Fallback/>
-  </mc:AlternateContent>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:twoCellAnchor editAs="oneCell">
-        <xdr:from>
-          <xdr:col>6</xdr:col>
-          <xdr:colOff>28575</xdr:colOff>
           <xdr:row>56</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
@@ -34319,14 +34248,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>6</xdr:col>
           <xdr:colOff>28575</xdr:colOff>
           <xdr:row>86</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="228600" cy="209550"/>
+        <xdr:to>
+          <xdr:col>6</xdr:col>
+          <xdr:colOff>257175</xdr:colOff>
+          <xdr:row>88</xdr:row>
+          <xdr:rowOff>19050</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1543" name="Check Box 519" hidden="1">
@@ -34372,7 +34306,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -34700,7 +34634,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
+      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -34766,7 +34700,7 @@
       </c>
       <c r="B3" s="16">
         <f>COUNTIFS(E:AI,FALSE)</f>
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="AJ3">
         <v>0.1</v>
@@ -34801,50 +34735,50 @@
       <c r="B7" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D7" s="25"/>
-      <c r="F7" s="24" t="s">
+      <c r="D7" s="29"/>
+      <c r="F7" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="I7" s="24" t="s">
+      <c r="G7" s="29"/>
+      <c r="I7" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="J7" s="25"/>
-      <c r="L7" s="24" t="s">
+      <c r="J7" s="29"/>
+      <c r="L7" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="M7" s="25"/>
-      <c r="O7" s="24" t="s">
+      <c r="M7" s="29"/>
+      <c r="O7" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="P7" s="25"/>
-      <c r="R7" s="24" t="s">
+      <c r="P7" s="29"/>
+      <c r="R7" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="S7" s="25"/>
-      <c r="U7" s="24" t="s">
+      <c r="S7" s="29"/>
+      <c r="U7" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="V7" s="25"/>
-      <c r="X7" s="24" t="s">
+      <c r="V7" s="29"/>
+      <c r="X7" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="Y7" s="25"/>
-      <c r="AA7" s="24" t="s">
+      <c r="Y7" s="29"/>
+      <c r="AA7" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="AB7" s="25"/>
-      <c r="AD7" s="24" t="s">
+      <c r="AB7" s="29"/>
+      <c r="AD7" s="28" t="s">
         <v>96</v>
       </c>
-      <c r="AE7" s="25"/>
-      <c r="AG7" s="24" t="s">
+      <c r="AE7" s="29"/>
+      <c r="AG7" s="28" t="s">
         <v>97</v>
       </c>
-      <c r="AH7" s="25"/>
+      <c r="AH7" s="29"/>
       <c r="AJ7">
         <v>0.3</v>
       </c>
@@ -34863,13 +34797,9 @@
       <c r="E8" s="1" t="b">
         <v>0</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>176</v>
-      </c>
+      <c r="F8" s="8"/>
       <c r="G8" s="9"/>
-      <c r="H8" s="1" t="b">
-        <v>0</v>
-      </c>
+      <c r="H8" s="1"/>
       <c r="I8" s="8"/>
       <c r="J8" s="9"/>
       <c r="K8" s="1"/>
@@ -36141,10 +36071,10 @@
       <c r="AH36" s="5"/>
     </row>
     <row r="37" spans="1:34">
-      <c r="A37" s="26" t="s">
-        <v>186</v>
-      </c>
-      <c r="B37" s="28" t="s">
+      <c r="A37" s="24" t="s">
+        <v>185</v>
+      </c>
+      <c r="B37" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C37" s="8" t="s">
@@ -36211,8 +36141,8 @@
       <c r="AH37" s="5"/>
     </row>
     <row r="38" spans="1:34">
-      <c r="A38" s="27"/>
-      <c r="B38" s="29"/>
+      <c r="A38" s="25"/>
+      <c r="B38" s="27"/>
       <c r="C38" s="8" t="s">
         <v>141</v>
       </c>
@@ -36473,7 +36403,7 @@
     </row>
     <row r="43" spans="1:34">
       <c r="A43" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B43" s="13" t="s">
         <v>59</v>
@@ -37137,7 +37067,7 @@
         <v>0</v>
       </c>
       <c r="F58" s="8" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G58" s="5"/>
       <c r="H58" s="1" t="b">
@@ -37314,10 +37244,10 @@
       <c r="AH61" s="5"/>
     </row>
     <row r="62" spans="1:34">
-      <c r="A62" s="26" t="s">
+      <c r="A62" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="B62" s="28" t="s">
+      <c r="B62" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C62" s="8" t="s">
@@ -37384,8 +37314,8 @@
       <c r="AH62" s="5"/>
     </row>
     <row r="63" spans="1:34">
-      <c r="A63" s="27"/>
-      <c r="B63" s="29"/>
+      <c r="A63" s="25"/>
+      <c r="B63" s="27"/>
       <c r="C63" s="8" t="s">
         <v>141</v>
       </c>
@@ -37455,10 +37385,10 @@
       <c r="AH63" s="5"/>
     </row>
     <row r="64" spans="1:34">
-      <c r="A64" s="26" t="s">
+      <c r="A64" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="B64" s="28" t="s">
+      <c r="B64" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C64" s="8" t="s">
@@ -37525,8 +37455,8 @@
       <c r="AH64" s="5"/>
     </row>
     <row r="65" spans="1:34">
-      <c r="A65" s="27"/>
-      <c r="B65" s="29"/>
+      <c r="A65" s="25"/>
+      <c r="B65" s="27"/>
       <c r="C65" s="8" t="s">
         <v>141</v>
       </c>
@@ -38205,10 +38135,10 @@
       <c r="AH80" s="5"/>
     </row>
     <row r="81" spans="1:34">
-      <c r="A81" s="26" t="s">
+      <c r="A81" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="B81" s="28" t="s">
+      <c r="B81" s="26" t="s">
         <v>38</v>
       </c>
       <c r="C81" s="8" t="s">
@@ -38275,8 +38205,8 @@
       <c r="AH81" s="5"/>
     </row>
     <row r="82" spans="1:34">
-      <c r="A82" s="27"/>
-      <c r="B82" s="29"/>
+      <c r="A82" s="25"/>
+      <c r="B82" s="27"/>
       <c r="C82" s="8" t="s">
         <v>149</v>
       </c>
@@ -38553,7 +38483,7 @@
         <v>0</v>
       </c>
       <c r="F88" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G88" s="5"/>
       <c r="H88" s="1" t="b">
@@ -38582,42 +38512,42 @@
       <c r="AH88" s="5"/>
     </row>
     <row r="89" spans="1:34">
-      <c r="A89" s="26" t="s">
+      <c r="A89" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="B89" s="28" t="s">
+      <c r="B89" s="26" t="s">
         <v>58</v>
       </c>
       <c r="C89" s="8" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D89" s="5"/>
       <c r="E89" s="1" t="b">
         <v>0</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="G89" s="5"/>
       <c r="H89" s="1" t="b">
         <v>0</v>
       </c>
       <c r="I89" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="J89" s="5"/>
       <c r="K89" s="1" t="b">
         <v>0</v>
       </c>
       <c r="L89" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="M89" s="5"/>
       <c r="N89" s="1" t="b">
         <v>0</v>
       </c>
       <c r="O89" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="P89" s="5"/>
       <c r="Q89" s="1" t="b">
@@ -38631,21 +38561,21 @@
         <v>0</v>
       </c>
       <c r="U89" s="8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="V89" s="5"/>
       <c r="W89" t="b">
         <v>0</v>
       </c>
       <c r="X89" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="Y89" s="5"/>
       <c r="Z89" t="b">
         <v>0</v>
       </c>
       <c r="AA89" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AB89" s="5"/>
       <c r="AC89" t="b">
@@ -38657,8 +38587,8 @@
       <c r="AH89" s="5"/>
     </row>
     <row r="90" spans="1:34">
-      <c r="A90" s="27"/>
-      <c r="B90" s="29"/>
+      <c r="A90" s="25"/>
+      <c r="B90" s="27"/>
       <c r="C90" s="8" t="s">
         <v>92</v>
       </c>
@@ -38781,7 +38711,7 @@
         <v>0</v>
       </c>
       <c r="F92" s="8" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G92" s="5"/>
       <c r="H92" s="1" t="b">
@@ -38849,10 +38779,10 @@
       <c r="AH93" s="5"/>
     </row>
     <row r="94" spans="1:34">
-      <c r="A94" s="26" t="s">
+      <c r="A94" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B94" s="28" t="s">
+      <c r="B94" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C94" s="8" t="s">
@@ -38919,8 +38849,8 @@
       <c r="AH94" s="5"/>
     </row>
     <row r="95" spans="1:34">
-      <c r="A95" s="27"/>
-      <c r="B95" s="29"/>
+      <c r="A95" s="25"/>
+      <c r="B95" s="27"/>
       <c r="C95" s="8" t="s">
         <v>149</v>
       </c>
@@ -39020,15 +38950,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="B94:B95"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A89:A90"/>
-    <mergeCell ref="B89:B90"/>
     <mergeCell ref="X7:Y7"/>
     <mergeCell ref="AA7:AB7"/>
     <mergeCell ref="AD7:AE7"/>
@@ -39043,6 +38964,15 @@
     <mergeCell ref="R7:S7"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="A94:A95"/>
+    <mergeCell ref="B94:B95"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A89:A90"/>
+    <mergeCell ref="B89:B90"/>
   </mergeCells>
   <conditionalFormatting sqref="C8:C96">
     <cfRule type="expression" dxfId="38" priority="39">
@@ -46116,29 +46046,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1444" r:id="rId318" name="Check Box 420">
-              <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
-                <anchor moveWithCells="1">
-                  <from>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>28575</xdr:colOff>
-                    <xdr:row>6</xdr:row>
-                    <xdr:rowOff>171450</xdr:rowOff>
-                  </from>
-                  <to>
-                    <xdr:col>6</xdr:col>
-                    <xdr:colOff>257175</xdr:colOff>
-                    <xdr:row>8</xdr:row>
-                    <xdr:rowOff>9525</xdr:rowOff>
-                  </to>
-                </anchor>
-              </controlPr>
-            </control>
-          </mc:Choice>
-        </mc:AlternateContent>
-        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-          <mc:Choice Requires="x14">
-            <control shapeId="1445" r:id="rId319" name="Check Box 421">
+            <control shapeId="1445" r:id="rId318" name="Check Box 421">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46160,7 +46068,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1446" r:id="rId320" name="Check Box 422">
+            <control shapeId="1446" r:id="rId319" name="Check Box 422">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46182,7 +46090,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1447" r:id="rId321" name="Check Box 423">
+            <control shapeId="1447" r:id="rId320" name="Check Box 423">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46204,7 +46112,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1448" r:id="rId322" name="Check Box 424">
+            <control shapeId="1448" r:id="rId321" name="Check Box 424">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46226,7 +46134,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1449" r:id="rId323" name="Check Box 425">
+            <control shapeId="1449" r:id="rId322" name="Check Box 425">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46248,7 +46156,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1232" r:id="rId324" name="Check Box 208">
+            <control shapeId="1232" r:id="rId323" name="Check Box 208">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46270,7 +46178,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1450" r:id="rId325" name="Check Box 426">
+            <control shapeId="1450" r:id="rId324" name="Check Box 426">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46292,7 +46200,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1230" r:id="rId326" name="Check Box 206">
+            <control shapeId="1230" r:id="rId325" name="Check Box 206">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46314,7 +46222,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1231" r:id="rId327" name="Check Box 207">
+            <control shapeId="1231" r:id="rId326" name="Check Box 207">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46336,7 +46244,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1451" r:id="rId328" name="Check Box 427">
+            <control shapeId="1451" r:id="rId327" name="Check Box 427">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46358,7 +46266,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1452" r:id="rId329" name="Check Box 428">
+            <control shapeId="1452" r:id="rId328" name="Check Box 428">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46380,7 +46288,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1454" r:id="rId330" name="Check Box 430">
+            <control shapeId="1454" r:id="rId329" name="Check Box 430">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46402,7 +46310,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1275" r:id="rId331" name="Check Box 251">
+            <control shapeId="1275" r:id="rId330" name="Check Box 251">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46424,7 +46332,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1276" r:id="rId332" name="Check Box 252">
+            <control shapeId="1276" r:id="rId331" name="Check Box 252">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46446,7 +46354,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1453" r:id="rId333" name="Check Box 429">
+            <control shapeId="1453" r:id="rId332" name="Check Box 429">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46468,7 +46376,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1456" r:id="rId334" name="Check Box 432">
+            <control shapeId="1456" r:id="rId333" name="Check Box 432">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46490,7 +46398,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1306" r:id="rId335" name="Check Box 282">
+            <control shapeId="1306" r:id="rId334" name="Check Box 282">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46512,7 +46420,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1307" r:id="rId336" name="Check Box 283">
+            <control shapeId="1307" r:id="rId335" name="Check Box 283">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46534,7 +46442,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1455" r:id="rId337" name="Check Box 431">
+            <control shapeId="1455" r:id="rId336" name="Check Box 431">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46556,7 +46464,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1458" r:id="rId338" name="Check Box 434">
+            <control shapeId="1458" r:id="rId337" name="Check Box 434">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46578,7 +46486,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1335" r:id="rId339" name="Check Box 311">
+            <control shapeId="1335" r:id="rId338" name="Check Box 311">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46600,7 +46508,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1336" r:id="rId340" name="Check Box 312">
+            <control shapeId="1336" r:id="rId339" name="Check Box 312">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46622,7 +46530,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1457" r:id="rId341" name="Check Box 433">
+            <control shapeId="1457" r:id="rId340" name="Check Box 433">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46644,7 +46552,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1460" r:id="rId342" name="Check Box 436">
+            <control shapeId="1460" r:id="rId341" name="Check Box 436">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46666,7 +46574,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1360" r:id="rId343" name="Check Box 336">
+            <control shapeId="1360" r:id="rId342" name="Check Box 336">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46688,7 +46596,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1361" r:id="rId344" name="Check Box 337">
+            <control shapeId="1361" r:id="rId343" name="Check Box 337">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46710,7 +46618,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1459" r:id="rId345" name="Check Box 435">
+            <control shapeId="1459" r:id="rId344" name="Check Box 435">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46732,7 +46640,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1462" r:id="rId346" name="Check Box 438">
+            <control shapeId="1462" r:id="rId345" name="Check Box 438">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46754,7 +46662,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1389" r:id="rId347" name="Check Box 365">
+            <control shapeId="1389" r:id="rId346" name="Check Box 365">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46776,7 +46684,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1390" r:id="rId348" name="Check Box 366">
+            <control shapeId="1390" r:id="rId347" name="Check Box 366">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46798,7 +46706,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1461" r:id="rId349" name="Check Box 437">
+            <control shapeId="1461" r:id="rId348" name="Check Box 437">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46820,7 +46728,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1464" r:id="rId350" name="Check Box 440">
+            <control shapeId="1464" r:id="rId349" name="Check Box 440">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46842,7 +46750,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1395" r:id="rId351" name="Check Box 371">
+            <control shapeId="1395" r:id="rId350" name="Check Box 371">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46864,7 +46772,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1396" r:id="rId352" name="Check Box 372">
+            <control shapeId="1396" r:id="rId351" name="Check Box 372">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46886,7 +46794,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1463" r:id="rId353" name="Check Box 439">
+            <control shapeId="1463" r:id="rId352" name="Check Box 439">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46908,7 +46816,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1466" r:id="rId354" name="Check Box 442">
+            <control shapeId="1466" r:id="rId353" name="Check Box 442">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46930,7 +46838,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1224" r:id="rId355" name="Check Box 200">
+            <control shapeId="1224" r:id="rId354" name="Check Box 200">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46952,7 +46860,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1225" r:id="rId356" name="Check Box 201">
+            <control shapeId="1225" r:id="rId355" name="Check Box 201">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46974,7 +46882,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1467" r:id="rId357" name="Check Box 443">
+            <control shapeId="1467" r:id="rId356" name="Check Box 443">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -46996,7 +46904,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1269" r:id="rId358" name="Check Box 245">
+            <control shapeId="1269" r:id="rId357" name="Check Box 245">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47018,7 +46926,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1270" r:id="rId359" name="Check Box 246">
+            <control shapeId="1270" r:id="rId358" name="Check Box 246">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47040,7 +46948,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1468" r:id="rId360" name="Check Box 444">
+            <control shapeId="1468" r:id="rId359" name="Check Box 444">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47062,7 +46970,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1469" r:id="rId361" name="Check Box 445">
+            <control shapeId="1469" r:id="rId360" name="Check Box 445">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47084,7 +46992,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1470" r:id="rId362" name="Check Box 446">
+            <control shapeId="1470" r:id="rId361" name="Check Box 446">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47106,7 +47014,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1471" r:id="rId363" name="Check Box 447">
+            <control shapeId="1471" r:id="rId362" name="Check Box 447">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47128,7 +47036,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1473" r:id="rId364" name="Check Box 449">
+            <control shapeId="1473" r:id="rId363" name="Check Box 449">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47150,7 +47058,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1286" r:id="rId365" name="Check Box 262">
+            <control shapeId="1286" r:id="rId364" name="Check Box 262">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47172,7 +47080,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1474" r:id="rId366" name="Check Box 450">
+            <control shapeId="1474" r:id="rId365" name="Check Box 450">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47194,7 +47102,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1475" r:id="rId367" name="Check Box 451">
+            <control shapeId="1475" r:id="rId366" name="Check Box 451">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47216,7 +47124,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1476" r:id="rId368" name="Check Box 452">
+            <control shapeId="1476" r:id="rId367" name="Check Box 452">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47238,7 +47146,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1477" r:id="rId369" name="Check Box 453">
+            <control shapeId="1477" r:id="rId368" name="Check Box 453">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47260,7 +47168,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1478" r:id="rId370" name="Check Box 454">
+            <control shapeId="1478" r:id="rId369" name="Check Box 454">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47282,7 +47190,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1309" r:id="rId371" name="Check Box 285">
+            <control shapeId="1309" r:id="rId370" name="Check Box 285">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47304,7 +47212,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1310" r:id="rId372" name="Check Box 286">
+            <control shapeId="1310" r:id="rId371" name="Check Box 286">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47326,7 +47234,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1311" r:id="rId373" name="Check Box 287">
+            <control shapeId="1311" r:id="rId372" name="Check Box 287">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47348,7 +47256,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1312" r:id="rId374" name="Check Box 288">
+            <control shapeId="1312" r:id="rId373" name="Check Box 288">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47370,7 +47278,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1313" r:id="rId375" name="Check Box 289">
+            <control shapeId="1313" r:id="rId374" name="Check Box 289">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47392,7 +47300,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1314" r:id="rId376" name="Check Box 290">
+            <control shapeId="1314" r:id="rId375" name="Check Box 290">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47414,7 +47322,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1315" r:id="rId377" name="Check Box 291">
+            <control shapeId="1315" r:id="rId376" name="Check Box 291">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47436,7 +47344,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1316" r:id="rId378" name="Check Box 292">
+            <control shapeId="1316" r:id="rId377" name="Check Box 292">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47458,7 +47366,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1479" r:id="rId379" name="Check Box 455">
+            <control shapeId="1479" r:id="rId378" name="Check Box 455">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47480,7 +47388,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1480" r:id="rId380" name="Check Box 456">
+            <control shapeId="1480" r:id="rId379" name="Check Box 456">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47502,7 +47410,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1481" r:id="rId381" name="Check Box 457">
+            <control shapeId="1481" r:id="rId380" name="Check Box 457">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47524,7 +47432,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1482" r:id="rId382" name="Check Box 458">
+            <control shapeId="1482" r:id="rId381" name="Check Box 458">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47546,7 +47454,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1483" r:id="rId383" name="Check Box 459">
+            <control shapeId="1483" r:id="rId382" name="Check Box 459">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47568,7 +47476,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1484" r:id="rId384" name="Check Box 460">
+            <control shapeId="1484" r:id="rId383" name="Check Box 460">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47590,7 +47498,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1485" r:id="rId385" name="Check Box 461">
+            <control shapeId="1485" r:id="rId384" name="Check Box 461">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47612,7 +47520,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1486" r:id="rId386" name="Check Box 462">
+            <control shapeId="1486" r:id="rId385" name="Check Box 462">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47634,7 +47542,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1337" r:id="rId387" name="Check Box 313">
+            <control shapeId="1337" r:id="rId386" name="Check Box 313">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47656,7 +47564,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1338" r:id="rId388" name="Check Box 314">
+            <control shapeId="1338" r:id="rId387" name="Check Box 314">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47678,7 +47586,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1339" r:id="rId389" name="Check Box 315">
+            <control shapeId="1339" r:id="rId388" name="Check Box 315">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47700,7 +47608,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1340" r:id="rId390" name="Check Box 316">
+            <control shapeId="1340" r:id="rId389" name="Check Box 316">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47722,7 +47630,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1341" r:id="rId391" name="Check Box 317">
+            <control shapeId="1341" r:id="rId390" name="Check Box 317">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47744,7 +47652,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1342" r:id="rId392" name="Check Box 318">
+            <control shapeId="1342" r:id="rId391" name="Check Box 318">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47766,7 +47674,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1343" r:id="rId393" name="Check Box 319">
+            <control shapeId="1343" r:id="rId392" name="Check Box 319">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47788,7 +47696,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1344" r:id="rId394" name="Check Box 320">
+            <control shapeId="1344" r:id="rId393" name="Check Box 320">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47810,7 +47718,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1487" r:id="rId395" name="Check Box 463">
+            <control shapeId="1487" r:id="rId394" name="Check Box 463">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47832,7 +47740,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1488" r:id="rId396" name="Check Box 464">
+            <control shapeId="1488" r:id="rId395" name="Check Box 464">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47854,7 +47762,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1489" r:id="rId397" name="Check Box 465">
+            <control shapeId="1489" r:id="rId396" name="Check Box 465">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47876,7 +47784,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1490" r:id="rId398" name="Check Box 466">
+            <control shapeId="1490" r:id="rId397" name="Check Box 466">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47898,7 +47806,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1362" r:id="rId399" name="Check Box 338">
+            <control shapeId="1362" r:id="rId398" name="Check Box 338">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47920,7 +47828,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1363" r:id="rId400" name="Check Box 339">
+            <control shapeId="1363" r:id="rId399" name="Check Box 339">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47942,7 +47850,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1364" r:id="rId401" name="Check Box 340">
+            <control shapeId="1364" r:id="rId400" name="Check Box 340">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47964,7 +47872,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1365" r:id="rId402" name="Check Box 341">
+            <control shapeId="1365" r:id="rId401" name="Check Box 341">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -47986,7 +47894,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1366" r:id="rId403" name="Check Box 342">
+            <control shapeId="1366" r:id="rId402" name="Check Box 342">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48008,7 +47916,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1367" r:id="rId404" name="Check Box 343">
+            <control shapeId="1367" r:id="rId403" name="Check Box 343">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48030,7 +47938,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1368" r:id="rId405" name="Check Box 344">
+            <control shapeId="1368" r:id="rId404" name="Check Box 344">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48052,7 +47960,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1369" r:id="rId406" name="Check Box 345">
+            <control shapeId="1369" r:id="rId405" name="Check Box 345">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48074,7 +47982,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1491" r:id="rId407" name="Check Box 467">
+            <control shapeId="1491" r:id="rId406" name="Check Box 467">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48096,7 +48004,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1492" r:id="rId408" name="Check Box 468">
+            <control shapeId="1492" r:id="rId407" name="Check Box 468">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48118,7 +48026,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1493" r:id="rId409" name="Check Box 469">
+            <control shapeId="1493" r:id="rId408" name="Check Box 469">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48140,7 +48048,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1494" r:id="rId410" name="Check Box 470">
+            <control shapeId="1494" r:id="rId409" name="Check Box 470">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48162,7 +48070,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1495" r:id="rId411" name="Check Box 471">
+            <control shapeId="1495" r:id="rId410" name="Check Box 471">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48184,7 +48092,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1496" r:id="rId412" name="Check Box 472">
+            <control shapeId="1496" r:id="rId411" name="Check Box 472">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48206,7 +48114,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1497" r:id="rId413" name="Check Box 473">
+            <control shapeId="1497" r:id="rId412" name="Check Box 473">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48228,7 +48136,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1498" r:id="rId414" name="Check Box 474">
+            <control shapeId="1498" r:id="rId413" name="Check Box 474">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48250,7 +48158,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1499" r:id="rId415" name="Check Box 475">
+            <control shapeId="1499" r:id="rId414" name="Check Box 475">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48272,7 +48180,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1500" r:id="rId416" name="Check Box 476">
+            <control shapeId="1500" r:id="rId415" name="Check Box 476">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48294,7 +48202,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1501" r:id="rId417" name="Check Box 477">
+            <control shapeId="1501" r:id="rId416" name="Check Box 477">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48316,7 +48224,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1502" r:id="rId418" name="Check Box 478">
+            <control shapeId="1502" r:id="rId417" name="Check Box 478">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48338,7 +48246,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1503" r:id="rId419" name="Check Box 479">
+            <control shapeId="1503" r:id="rId418" name="Check Box 479">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48360,7 +48268,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1504" r:id="rId420" name="Check Box 480">
+            <control shapeId="1504" r:id="rId419" name="Check Box 480">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48382,7 +48290,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1505" r:id="rId421" name="Check Box 481">
+            <control shapeId="1505" r:id="rId420" name="Check Box 481">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48404,7 +48312,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1506" r:id="rId422" name="Check Box 482">
+            <control shapeId="1506" r:id="rId421" name="Check Box 482">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48426,7 +48334,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1398" r:id="rId423" name="Check Box 374">
+            <control shapeId="1398" r:id="rId422" name="Check Box 374">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48448,7 +48356,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1399" r:id="rId424" name="Check Box 375">
+            <control shapeId="1399" r:id="rId423" name="Check Box 375">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48470,7 +48378,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1400" r:id="rId425" name="Check Box 376">
+            <control shapeId="1400" r:id="rId424" name="Check Box 376">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48492,7 +48400,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1401" r:id="rId426" name="Check Box 377">
+            <control shapeId="1401" r:id="rId425" name="Check Box 377">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48514,7 +48422,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1402" r:id="rId427" name="Check Box 378">
+            <control shapeId="1402" r:id="rId426" name="Check Box 378">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48536,7 +48444,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1403" r:id="rId428" name="Check Box 379">
+            <control shapeId="1403" r:id="rId427" name="Check Box 379">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48558,7 +48466,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1404" r:id="rId429" name="Check Box 380">
+            <control shapeId="1404" r:id="rId428" name="Check Box 380">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48580,7 +48488,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1405" r:id="rId430" name="Check Box 381">
+            <control shapeId="1405" r:id="rId429" name="Check Box 381">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48602,7 +48510,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1418" r:id="rId431" name="Check Box 394">
+            <control shapeId="1418" r:id="rId430" name="Check Box 394">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48624,7 +48532,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1419" r:id="rId432" name="Check Box 395">
+            <control shapeId="1419" r:id="rId431" name="Check Box 395">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48646,7 +48554,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1420" r:id="rId433" name="Check Box 396">
+            <control shapeId="1420" r:id="rId432" name="Check Box 396">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48668,7 +48576,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1421" r:id="rId434" name="Check Box 397">
+            <control shapeId="1421" r:id="rId433" name="Check Box 397">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48690,7 +48598,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1507" r:id="rId435" name="Check Box 483">
+            <control shapeId="1507" r:id="rId434" name="Check Box 483">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48712,7 +48620,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1508" r:id="rId436" name="Check Box 484">
+            <control shapeId="1508" r:id="rId435" name="Check Box 484">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48734,7 +48642,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1509" r:id="rId437" name="Check Box 485">
+            <control shapeId="1509" r:id="rId436" name="Check Box 485">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48756,7 +48664,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1510" r:id="rId438" name="Check Box 486">
+            <control shapeId="1510" r:id="rId437" name="Check Box 486">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48778,7 +48686,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1511" r:id="rId439" name="Check Box 487">
+            <control shapeId="1511" r:id="rId438" name="Check Box 487">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48800,7 +48708,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1512" r:id="rId440" name="Check Box 488">
+            <control shapeId="1512" r:id="rId439" name="Check Box 488">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48822,7 +48730,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1513" r:id="rId441" name="Check Box 489">
+            <control shapeId="1513" r:id="rId440" name="Check Box 489">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48844,7 +48752,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1514" r:id="rId442" name="Check Box 490">
+            <control shapeId="1514" r:id="rId441" name="Check Box 490">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48866,7 +48774,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1465" r:id="rId443" name="Check Box 441">
+            <control shapeId="1465" r:id="rId442" name="Check Box 441">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48888,7 +48796,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1515" r:id="rId444" name="Check Box 491">
+            <control shapeId="1515" r:id="rId443" name="Check Box 491">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48910,7 +48818,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1516" r:id="rId445" name="Check Box 492">
+            <control shapeId="1516" r:id="rId444" name="Check Box 492">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48932,7 +48840,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1517" r:id="rId446" name="Check Box 493">
+            <control shapeId="1517" r:id="rId445" name="Check Box 493">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48954,7 +48862,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1518" r:id="rId447" name="Check Box 494">
+            <control shapeId="1518" r:id="rId446" name="Check Box 494">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48976,7 +48884,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1217" r:id="rId448" name="Check Box 193">
+            <control shapeId="1217" r:id="rId447" name="Check Box 193">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -48998,7 +48906,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1519" r:id="rId449" name="Check Box 495">
+            <control shapeId="1519" r:id="rId448" name="Check Box 495">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49020,7 +48928,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1520" r:id="rId450" name="Check Box 496">
+            <control shapeId="1520" r:id="rId449" name="Check Box 496">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49042,7 +48950,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1521" r:id="rId451" name="Check Box 497">
+            <control shapeId="1521" r:id="rId450" name="Check Box 497">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49064,7 +48972,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1522" r:id="rId452" name="Check Box 498">
+            <control shapeId="1522" r:id="rId451" name="Check Box 498">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49086,7 +48994,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1262" r:id="rId453" name="Check Box 238">
+            <control shapeId="1262" r:id="rId452" name="Check Box 238">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49108,7 +49016,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1523" r:id="rId454" name="Check Box 499">
+            <control shapeId="1523" r:id="rId453" name="Check Box 499">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49130,7 +49038,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1297" r:id="rId455" name="Check Box 273">
+            <control shapeId="1297" r:id="rId454" name="Check Box 273">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49152,7 +49060,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1524" r:id="rId456" name="Check Box 500">
+            <control shapeId="1524" r:id="rId455" name="Check Box 500">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49174,7 +49082,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1328" r:id="rId457" name="Check Box 304">
+            <control shapeId="1328" r:id="rId456" name="Check Box 304">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49196,7 +49104,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1525" r:id="rId458" name="Check Box 501">
+            <control shapeId="1525" r:id="rId457" name="Check Box 501">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49218,7 +49126,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1526" r:id="rId459" name="Check Box 502">
+            <control shapeId="1526" r:id="rId458" name="Check Box 502">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49240,7 +49148,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1527" r:id="rId460" name="Check Box 503">
+            <control shapeId="1527" r:id="rId459" name="Check Box 503">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49262,7 +49170,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1354" r:id="rId461" name="Check Box 330">
+            <control shapeId="1354" r:id="rId460" name="Check Box 330">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49284,7 +49192,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1528" r:id="rId462" name="Check Box 504">
+            <control shapeId="1528" r:id="rId461" name="Check Box 504">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49306,7 +49214,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1529" r:id="rId463" name="Check Box 505">
+            <control shapeId="1529" r:id="rId462" name="Check Box 505">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49328,7 +49236,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1383" r:id="rId464" name="Check Box 359">
+            <control shapeId="1383" r:id="rId463" name="Check Box 359">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49350,7 +49258,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1530" r:id="rId465" name="Check Box 506">
+            <control shapeId="1530" r:id="rId464" name="Check Box 506">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49372,7 +49280,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1531" r:id="rId466" name="Check Box 507">
+            <control shapeId="1531" r:id="rId465" name="Check Box 507">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49394,7 +49302,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1532" r:id="rId467" name="Check Box 508">
+            <control shapeId="1532" r:id="rId466" name="Check Box 508">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49416,7 +49324,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1533" r:id="rId468" name="Check Box 509">
+            <control shapeId="1533" r:id="rId467" name="Check Box 509">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49438,7 +49346,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1534" r:id="rId469" name="Check Box 510">
+            <control shapeId="1534" r:id="rId468" name="Check Box 510">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49460,7 +49368,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1391" r:id="rId470" name="Check Box 367">
+            <control shapeId="1391" r:id="rId469" name="Check Box 367">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49482,7 +49390,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1392" r:id="rId471" name="Check Box 368">
+            <control shapeId="1392" r:id="rId470" name="Check Box 368">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49504,7 +49412,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1393" r:id="rId472" name="Check Box 369">
+            <control shapeId="1393" r:id="rId471" name="Check Box 369">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49526,7 +49434,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1394" r:id="rId473" name="Check Box 370">
+            <control shapeId="1394" r:id="rId472" name="Check Box 370">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49548,7 +49456,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1535" r:id="rId474" name="Check Box 511">
+            <control shapeId="1535" r:id="rId473" name="Check Box 511">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49570,7 +49478,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1536" r:id="rId475" name="Check Box 512">
+            <control shapeId="1536" r:id="rId474" name="Check Box 512">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49592,7 +49500,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1537" r:id="rId476" name="Check Box 513">
+            <control shapeId="1537" r:id="rId475" name="Check Box 513">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49614,7 +49522,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1538" r:id="rId477" name="Check Box 514">
+            <control shapeId="1538" r:id="rId476" name="Check Box 514">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49636,7 +49544,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1539" r:id="rId478" name="Check Box 515">
+            <control shapeId="1539" r:id="rId477" name="Check Box 515">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49658,7 +49566,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1397" r:id="rId479" name="Check Box 373">
+            <control shapeId="1397" r:id="rId478" name="Check Box 373">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49680,7 +49588,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1247" r:id="rId480" name="Check Box 223">
+            <control shapeId="1247" r:id="rId479" name="Check Box 223">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49702,7 +49610,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1472" r:id="rId481" name="Check Box 448">
+            <control shapeId="1472" r:id="rId480" name="Check Box 448">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49724,7 +49632,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1099" r:id="rId482" name="Check Box 75">
+            <control shapeId="1099" r:id="rId481" name="Check Box 75">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49746,7 +49654,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1100" r:id="rId483" name="Check Box 76">
+            <control shapeId="1100" r:id="rId482" name="Check Box 76">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49768,7 +49676,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1542" r:id="rId484" name="Check Box 518">
+            <control shapeId="1542" r:id="rId483" name="Check Box 518">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49790,7 +49698,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1541" r:id="rId485" name="Check Box 517">
+            <control shapeId="1541" r:id="rId484" name="Check Box 517">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
@@ -49812,7 +49720,7 @@
         </mc:AlternateContent>
         <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
           <mc:Choice Requires="x14">
-            <control shapeId="1543" r:id="rId486" name="Check Box 519">
+            <control shapeId="1543" r:id="rId485" name="Check Box 519">
               <controlPr defaultSize="0" autoFill="0" autoLine="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>

</xml_diff>